<commit_message>
Added Opening and Closing Hours, Connected to Tables page
</commit_message>
<xml_diff>
--- a/11111111111111/Customer Service.xlsx
+++ b/11111111111111/Customer Service.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,6 +415,72 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Table Number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Capacity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Occupied</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Table 1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Table 2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -424,17 +492,53 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Table Number</t>
+          <t>SNo</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Capacity</t>
+          <t>Dish</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Occupied</t>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited Error in Menu
</commit_message>
<xml_diff>
--- a/11111111111111/Customer Service.xlsx
+++ b/11111111111111/Customer Service.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Table 2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +435,237 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Occupied</t>
+          <t>00:00</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>00:30</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>01:00</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>01:30</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>02:00</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>02:30</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>03:00</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>03:30</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>04:00</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>04:30</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>05:00</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>05:30</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>06:00</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>06:30</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>07:00</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>07:30</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>08:30</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
+        <is>
+          <t>20:30</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>21:00</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>21:30</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>22:00</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>22:30</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>23:00</t>
         </is>
       </c>
     </row>
@@ -454,19 +683,142 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Table 2</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="b">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AU2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AV2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -509,40 +861,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>SNo</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Dish</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Customer Service Page
</commit_message>
<xml_diff>
--- a/11111111111111/Customer Service.xlsx
+++ b/11111111111111/Customer Service.xlsx
@@ -2,16 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Table 2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Table 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Table 4" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Table 5" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Table 6" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -51,7 +55,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,13 +418,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -435,37 +439,152 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>01:30</t>
+          <t>06:00</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>02:00</t>
+          <t>06:30</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>02:30</t>
+          <t>07:00</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>03:00</t>
+          <t>07:30</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>03:30</t>
+          <t>08:00</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>04:00</t>
+          <t>08:30</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>04:30</t>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>09:30</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>10:30</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>12:30</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>13:00</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>13:30</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>14:30</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>15:00</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>15:30</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>16:30</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>17:00</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>17:30</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>18:00</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>18:30</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>19:00</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>19:30</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>20:00</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>20:30</t>
         </is>
       </c>
     </row>
@@ -477,7 +596,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="b">
@@ -499,6 +618,585 @@
         <v>0</v>
       </c>
       <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="O2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <v>0</v>
+      </c>
+      <c r="V2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W2" t="b">
+        <v>0</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Table 2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <v>0</v>
+      </c>
+      <c r="U3" t="b">
+        <v>0</v>
+      </c>
+      <c r="V3" t="b">
+        <v>0</v>
+      </c>
+      <c r="W3" t="b">
+        <v>0</v>
+      </c>
+      <c r="X3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Table 3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>0</v>
+      </c>
+      <c r="T4" t="b">
+        <v>0</v>
+      </c>
+      <c r="U4" t="b">
+        <v>0</v>
+      </c>
+      <c r="V4" t="b">
+        <v>0</v>
+      </c>
+      <c r="W4" t="b">
+        <v>0</v>
+      </c>
+      <c r="X4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Table 4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Table 5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="b">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>0</v>
+      </c>
+      <c r="T6" t="b">
+        <v>0</v>
+      </c>
+      <c r="U6" t="b">
+        <v>0</v>
+      </c>
+      <c r="V6" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Table 6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>0</v>
+      </c>
+      <c r="O7" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" t="b">
+        <v>0</v>
+      </c>
+      <c r="U7" t="b">
+        <v>0</v>
+      </c>
+      <c r="V7" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -513,13 +1211,87 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -535,6 +1307,200 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>SNo</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Dish</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
         </is>
       </c>
     </row>

</xml_diff>